<commit_message>
Sherwin Miller Project Final
</commit_message>
<xml_diff>
--- a/Project_Draft/Morph Table for Evolution project.xlsx
+++ b/Project_Draft/Morph Table for Evolution project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sherm\Desktop\Evolution\Tasks\Projectremodified\Analysis_Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sherm\Desktop\Evolution\Tasks\Projectremodified\Project_Draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5ED80E-F7AF-4579-9540-D48364E6C91B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A52232E-3328-4B39-8080-0035507E3CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E704659-A9EB-426A-A134-4F3405BB87D4}"/>
   </bookViews>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65A00A4-844A-4551-AE43-6B823C6B8990}">
   <dimension ref="A1:G196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection sqref="A1:G196"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="I152" sqref="I152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>